<commit_message>
Adding automation script to scrapping proecesses in scripts folder
</commit_message>
<xml_diff>
--- a/dataSet/cleanData/missingDataValues.xlsx
+++ b/dataSet/cleanData/missingDataValues.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -479,7 +479,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -507,11 +507,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>population</t>
+          <t>stringency_index</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -523,49 +523,65 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Oporavljeni</t>
+          <t>population</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>231</v>
+        <v>308</v>
       </c>
       <c r="C6" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.329004329004329</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Testirani</t>
+          <t>Oporavljeni</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>231</v>
       </c>
       <c r="C7" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" t="n">
-        <v>0.329004329004329</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Testirani</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>231</v>
+      </c>
+      <c r="C8" t="n">
+        <v>77</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>Smrtni sl.</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B9" t="n">
         <v>232</v>
       </c>
-      <c r="C8" t="n">
-        <v>75</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.3232758620689655</v>
+      <c r="C9" t="n">
+        <v>76</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3275862068965517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parsing dataframe and adding it to the website
</commit_message>
<xml_diff>
--- a/dataSet/cleanData/missingDataValues.xlsx
+++ b/dataSet/cleanData/missingDataValues.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -479,7 +479,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -507,11 +507,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>stringency_index</t>
+          <t>population</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -523,65 +523,49 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>population</t>
+          <t>Oporavljeni</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>308</v>
+        <v>231</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.3376623376623377</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Oporavljeni</t>
+          <t>Testirani</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>231</v>
       </c>
       <c r="C7" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.3376623376623377</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Testirani</t>
+          <t>Smrtni sl.</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C8" t="n">
         <v>77</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Smrtni sl.</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>232</v>
-      </c>
-      <c r="C9" t="n">
-        <v>76</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.3275862068965517</v>
+        <v>0.331896551724138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>